<commit_message>
Toggle products table ok
</commit_message>
<xml_diff>
--- a/Proyecto_Integrador_-_Jugueteria_Cosmica_-_Etapa_3_-_Consignas_cumplidas.xlsx
+++ b/Proyecto_Integrador_-_Jugueteria_Cosmica_-_Etapa_3_-_Consignas_cumplidas.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
   <si>
     <r>
       <t xml:space="preserve">Proyecto Integrador: </t>
@@ -1381,13 +1381,19 @@
   </si>
   <si>
     <t>Se muestra en consola del servidor y también se almacena en la collection "productscarts"</t>
+  </si>
+  <si>
+    <t>Se definió el esquema del carrito también</t>
+  </si>
+  <si>
+    <t>https://github.com/gabymosci/aa-Proyecto-integrador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1472,6 +1478,14 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1510,11 +1524,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1548,9 +1563,11 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -1921,8 +1938,8 @@
   <dimension ref="A1:C135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C132" sqref="C132"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,6 +2938,9 @@
       <c r="B129" s="12" t="s">
         <v>130</v>
       </c>
+      <c r="C129" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="130" spans="1:3" ht="33" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
@@ -2955,6 +2975,9 @@
       </c>
       <c r="B133" s="12" t="s">
         <v>130</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
@@ -3007,7 +3030,10 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Solo &quot;Sí&quot; o &quot;No&quot;" error="Se debe ingresar exactamente &quot;Sí&quot; o &quot;No&quot;" sqref="B1"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C133" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tabla header y footer andando
</commit_message>
<xml_diff>
--- a/Proyecto_Integrador_-_Jugueteria_Cosmica_-_Etapa_3_-_Consignas_cumplidas.xlsx
+++ b/Proyecto_Integrador_-_Jugueteria_Cosmica_-_Etapa_3_-_Consignas_cumplidas.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="148">
   <si>
     <r>
       <t xml:space="preserve">Proyecto Integrador: </t>
@@ -1387,6 +1387,9 @@
   </si>
   <si>
     <t>https://github.com/gabymosci/aa-Proyecto-integrador</t>
+  </si>
+  <si>
+    <t>Usé una librería para la paginación obtenida de github</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1941,8 @@
   <dimension ref="A1:C135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,6 +2027,9 @@
       </c>
       <c r="B10" s="12" t="s">
         <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="66" x14ac:dyDescent="0.25">

</xml_diff>